<commit_message>
ready for merging with hp
</commit_message>
<xml_diff>
--- a/input/BatInput_prev.xlsx
+++ b/input/BatInput_prev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C38110-6D5F-49A9-B9DB-B92CEF633396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F44827-DD58-416B-A5A7-96E75B2C750B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2D6FB7A9-4863-426A-A67F-B0E64011A4E0}"/>
   </bookViews>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28622475-EB6F-4CD7-9A0D-9DFEA9718355}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,34 +735,8 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>26400</v>
-      </c>
-      <c r="C10" s="3">
-        <v>220</v>
-      </c>
-      <c r="D10">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3.66</v>
-      </c>
-      <c r="H10" s="1">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>